<commit_message>
updated ppt. added Aashu's part and corrected mine
</commit_message>
<xml_diff>
--- a/ResultGraphs/Aditya/Book.xlsx
+++ b/ResultGraphs/Aditya/Book.xlsx
@@ -110,6 +110,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1523,11 +1524,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84353408"/>
-        <c:axId val="84355712"/>
+        <c:axId val="86516096"/>
+        <c:axId val="86518400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84353408"/>
+        <c:axId val="86516096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1548,17 +1549,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84355712"/>
+        <c:crossAx val="86518400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84355712"/>
+        <c:axId val="86518400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1580,22 +1582,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84353408"/>
+        <c:crossAx val="86516096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1633,6 +1637,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3046,11 +3051,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84658432"/>
-        <c:axId val="84668800"/>
+        <c:axId val="86821120"/>
+        <c:axId val="86831488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84658432"/>
+        <c:axId val="86821120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3071,17 +3076,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84668800"/>
+        <c:crossAx val="86831488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84668800"/>
+        <c:axId val="86831488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3098,27 +3104,29 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number of Papers</a:t>
+                  <a:t>Number of Papers per Author</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84658432"/>
+        <c:crossAx val="86821120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4574,11 +4582,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84680704"/>
-        <c:axId val="84682624"/>
+        <c:axId val="86839296"/>
+        <c:axId val="86841216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84680704"/>
+        <c:axId val="86839296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4603,14 +4611,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84682624"/>
+        <c:crossAx val="86841216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84682624"/>
+        <c:axId val="86841216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4627,7 +4635,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number of Papers</a:t>
+                  <a:t>Number of Collaborators per Author</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4636,7 +4644,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84680704"/>
+        <c:crossAx val="86839296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4649,7 +4657,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4691,6 +4699,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -6104,11 +6113,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84833792"/>
-        <c:axId val="84835712"/>
+        <c:axId val="86996480"/>
+        <c:axId val="86998400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84833792"/>
+        <c:axId val="86996480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6129,17 +6138,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84835712"/>
+        <c:crossAx val="86998400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84835712"/>
+        <c:axId val="86998400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6156,27 +6166,29 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number of Papers</a:t>
+                  <a:t>Number of Single Authored Papers</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84833792"/>
+        <c:crossAx val="86996480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6392,139 +6404,139 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="45"/>
                 <c:pt idx="0">
-                  <c:v>2.5333332999999998</c:v>
+                  <c:v>0.39473686000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3199999999999998</c:v>
+                  <c:v>0.43103448</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5454545</c:v>
+                  <c:v>0.39285713</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.8333333000000001</c:v>
+                  <c:v>0.35294120000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>0.33333333999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6119403999999999</c:v>
+                  <c:v>0.38285713999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3797470000000001</c:v>
+                  <c:v>0.42021278000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.4729728999999998</c:v>
+                  <c:v>0.4043716</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.8985506999999999</c:v>
+                  <c:v>0.34499999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.8993289999999998</c:v>
+                  <c:v>0.34490739999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.0722222000000001</c:v>
+                  <c:v>0.32549729999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.8049792999999998</c:v>
+                  <c:v>0.35650887999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.2352940000000001</c:v>
+                  <c:v>0.3090909</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.9969969000000001</c:v>
+                  <c:v>0.33366733999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.9864407000000002</c:v>
+                  <c:v>0.33484676000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.2357724000000001</c:v>
+                  <c:v>0.30904523</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.3765903000000002</c:v>
+                  <c:v>0.29615672999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.3246074000000001</c:v>
+                  <c:v>0.30078739999999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.4949083000000001</c:v>
+                  <c:v>0.28613054999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.8297362000000001</c:v>
+                  <c:v>0.26111459999999997</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.5036900000000002</c:v>
+                  <c:v>0.28541337999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.4951612999999999</c:v>
+                  <c:v>0.28610983000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.5219939999999998</c:v>
+                  <c:v>0.28393005999999998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.5569334000000001</c:v>
+                  <c:v>0.28114104000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.5356394999999998</c:v>
+                  <c:v>0.28283426</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.6125702999999998</c:v>
+                  <c:v>0.27681119999999998</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.7420814</c:v>
+                  <c:v>0.26723096000000002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.635767</c:v>
+                  <c:v>0.27504513000000003</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.7050242</c:v>
+                  <c:v>0.26990375</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.8543753999999999</c:v>
+                  <c:v>0.25944539999999999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.6032926999999999</c:v>
+                  <c:v>0.27752396000000001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.7321996999999998</c:v>
+                  <c:v>0.26793850000000002</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.8033332999999998</c:v>
+                  <c:v>0.26292726</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.6797065999999998</c:v>
+                  <c:v>0.27176080000000002</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.8127870000000001</c:v>
+                  <c:v>0.26227534000000002</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.8323269999999998</c:v>
+                  <c:v>0.26093808000000002</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.9104682999999998</c:v>
+                  <c:v>0.25572382999999999</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.8405306000000001</c:v>
+                  <c:v>0.26038070000000002</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.1850265999999996</c:v>
+                  <c:v>0.2389471</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.0149125999999997</c:v>
+                  <c:v>0.24907141999999999</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.0448979999999999</c:v>
+                  <c:v>0.24722503000000001</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.0649569999999997</c:v>
+                  <c:v>0.24600504000000001</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.8371559999999998</c:v>
+                  <c:v>0.2606097</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.9621474999999999</c:v>
+                  <c:v>0.25238840000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6698,139 +6710,139 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="45"/>
                 <c:pt idx="0">
-                  <c:v>2.5333332999999998</c:v>
+                  <c:v>0.39473686000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3199999999999998</c:v>
+                  <c:v>0.43103448</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5454545</c:v>
+                  <c:v>0.39285713</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.8333333000000001</c:v>
+                  <c:v>0.35294120000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>0.33333333999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6666666999999999</c:v>
+                  <c:v>0.375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>0.43478260000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.4375</c:v>
+                  <c:v>0.41025642000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.3714284999999999</c:v>
+                  <c:v>0.42168674</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.7938930000000002</c:v>
+                  <c:v>0.35792350000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.8095238</c:v>
+                  <c:v>0.35593219999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.0620154999999998</c:v>
+                  <c:v>0.32658228</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.0337079</c:v>
+                  <c:v>0.32962963000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.2479339</c:v>
+                  <c:v>0.30788802999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.9761905999999998</c:v>
+                  <c:v>0.33600000000000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.8278690000000002</c:v>
+                  <c:v>0.35362317999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.4361700000000002</c:v>
+                  <c:v>0.29102167000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.3317757000000001</c:v>
+                  <c:v>0.30014025999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.3130841000000002</c:v>
+                  <c:v>0.30183357</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.521531</c:v>
+                  <c:v>0.28396739999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.0598802999999997</c:v>
+                  <c:v>0.24631268000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.2848835000000003</c:v>
+                  <c:v>0.23337856000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.8038278000000001</c:v>
+                  <c:v>0.26289308</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.9414634999999998</c:v>
+                  <c:v>0.25371285999999998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.7456445999999999</c:v>
+                  <c:v>0.26697673999999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.8357142999999998</c:v>
+                  <c:v>0.26070765000000001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.6088328000000001</c:v>
+                  <c:v>0.27709790000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.9520547000000001</c:v>
+                  <c:v>0.25303291999999999</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.9255664000000001</c:v>
+                  <c:v>0.25474033000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.9788519999999998</c:v>
+                  <c:v>0.25132876999999998</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.0144929999999999</c:v>
+                  <c:v>0.24909746999999999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.8223684000000002</c:v>
+                  <c:v>0.26161790000000001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.6928570000000001</c:v>
+                  <c:v>0.27079304999999998</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.7221375000000001</c:v>
+                  <c:v>0.26866284000000001</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.8064515999999999</c:v>
+                  <c:v>0.26271185000000002</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.9075066999999999</c:v>
+                  <c:v>0.25591766999999999</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.5622745</c:v>
+                  <c:v>0.28071954999999998</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.4588679999999998</c:v>
+                  <c:v>0.28911194000000001</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.8999079999999999</c:v>
+                  <c:v>0.25641629999999999</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.015625</c:v>
+                  <c:v>0.24902724000000001</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.8560688000000001</c:v>
+                  <c:v>0.25933146000000001</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3.6157205000000001</c:v>
+                  <c:v>0.27657005000000001</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.6031599999999999</c:v>
+                  <c:v>0.27753420000000001</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.4646466</c:v>
+                  <c:v>0.28862974000000002</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.6183866999999998</c:v>
+                  <c:v>0.27636625999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7004,103 +7016,103 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="45"/>
                 <c:pt idx="12">
-                  <c:v>2.1458333000000001</c:v>
+                  <c:v>0.46601942000000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.5211266999999999</c:v>
+                  <c:v>0.39664804999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.2045455</c:v>
+                  <c:v>0.45360824</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.3131312999999998</c:v>
+                  <c:v>0.43231439999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.0909089999999999</c:v>
+                  <c:v>0.47826087</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.3368419999999999</c:v>
+                  <c:v>0.42792794000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.3441296</c:v>
+                  <c:v>0.42659760000000002</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.3682432000000002</c:v>
+                  <c:v>0.42225393999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.4735203000000001</c:v>
+                  <c:v>0.40428212000000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.5269841999999998</c:v>
+                  <c:v>0.39572865000000002</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.5955284000000001</c:v>
+                  <c:v>0.38527800000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.6808510000000001</c:v>
+                  <c:v>0.37301588000000002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.0216799999999999</c:v>
+                  <c:v>0.33094170000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.9225807000000001</c:v>
+                  <c:v>0.34216334999999998</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.7206106000000001</c:v>
+                  <c:v>0.36756453</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.9703154999999999</c:v>
+                  <c:v>0.33666459999999998</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.9848275000000002</c:v>
+                  <c:v>0.33502771999999997</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.0013036999999998</c:v>
+                  <c:v>0.33318852999999998</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.0252100999999998</c:v>
+                  <c:v>0.33055556000000003</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.9572023999999999</c:v>
+                  <c:v>0.33815741999999999</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.9024165000000002</c:v>
+                  <c:v>0.34454050000000003</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.0810168</c:v>
+                  <c:v>0.32456817999999998</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.1145339999999999</c:v>
+                  <c:v>0.32107532</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.2113269999999998</c:v>
+                  <c:v>0.31139772999999998</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.9588087000000001</c:v>
+                  <c:v>0.33797386000000001</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.215856</c:v>
+                  <c:v>0.31095919999999999</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.3525143000000002</c:v>
+                  <c:v>0.29828359999999998</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3.3944223</c:v>
+                  <c:v>0.29460092999999998</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.4844176999999998</c:v>
+                  <c:v>0.28699197999999998</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.4211566000000002</c:v>
+                  <c:v>0.29229880000000003</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.5429417999999999</c:v>
+                  <c:v>0.28225133000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7274,103 +7286,103 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="45"/>
                 <c:pt idx="12">
-                  <c:v>2</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.1724138000000002</c:v>
+                  <c:v>0.46031746000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.2142856000000002</c:v>
+                  <c:v>0.45161289999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.4137930000000001</c:v>
+                  <c:v>0.41428572000000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.3333333000000001</c:v>
+                  <c:v>0.42857142999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.2666667</c:v>
+                  <c:v>0.44117646999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.0754716000000002</c:v>
+                  <c:v>0.48181816999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.347826</c:v>
+                  <c:v>0.42592594</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.2109375</c:v>
+                  <c:v>0.45229681999999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2424241999999999</c:v>
+                  <c:v>0.44594594999999998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.2962964000000001</c:v>
+                  <c:v>0.43548387</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.4976959999999999</c:v>
+                  <c:v>0.40036902000000002</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.4285714999999999</c:v>
+                  <c:v>0.41176469999999998</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.7363183000000002</c:v>
+                  <c:v>0.36545454999999999</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.4570637</c:v>
+                  <c:v>0.40698983999999999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.7349079999999999</c:v>
+                  <c:v>0.365643</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.8286853000000001</c:v>
+                  <c:v>0.35352114000000001</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.7438015999999998</c:v>
+                  <c:v>0.36445785000000003</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.8690095000000002</c:v>
+                  <c:v>0.34855235000000001</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.7867434000000002</c:v>
+                  <c:v>0.35884178</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.7741935</c:v>
+                  <c:v>0.36046509999999998</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.9435897</c:v>
+                  <c:v>0.33972126000000002</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.8509316</c:v>
+                  <c:v>0.35076252000000002</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.9965869999999999</c:v>
+                  <c:v>0.33371299999999998</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.8507042</c:v>
+                  <c:v>0.35079050000000001</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.7142856000000002</c:v>
+                  <c:v>0.36842105000000003</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3</c:v>
+                  <c:v>0.33333333999999998</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.7975078</c:v>
+                  <c:v>0.35746104000000001</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.8410852000000002</c:v>
+                  <c:v>0.35197817999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7544,99 +7556,99 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="45"/>
                 <c:pt idx="17">
-                  <c:v>2.0238094000000002</c:v>
+                  <c:v>0.49411765000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.1666666999999999</c:v>
+                  <c:v>0.46153845999999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.4166666999999999</c:v>
+                  <c:v>0.41379312000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.4166666999999999</c:v>
+                  <c:v>0.41379312000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.58</c:v>
+                  <c:v>0.38759690000000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.4264705000000002</c:v>
+                  <c:v>0.41212120000000002</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.8666665999999998</c:v>
+                  <c:v>0.34883720000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.359375</c:v>
+                  <c:v>0.42384105999999999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.3880596000000001</c:v>
+                  <c:v>0.41875000000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.4396550000000001</c:v>
+                  <c:v>0.40989399999999998</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.6129030000000002</c:v>
+                  <c:v>0.38271606000000002</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.4122447999999999</c:v>
+                  <c:v>0.41455162000000001</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.6898735</c:v>
+                  <c:v>0.37176471999999999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.5423453</c:v>
+                  <c:v>0.39333760000000001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.6825937999999998</c:v>
+                  <c:v>0.37277353000000002</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.5450081999999998</c:v>
+                  <c:v>0.39292603999999998</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.4640521999999998</c:v>
+                  <c:v>0.40583553999999999</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.6584506000000001</c:v>
+                  <c:v>0.37615894999999999</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.6355422000000002</c:v>
+                  <c:v>0.37942857000000002</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.4810894000000001</c:v>
+                  <c:v>0.40304878</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.6284290000000001</c:v>
+                  <c:v>0.3804554</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.7638888000000001</c:v>
+                  <c:v>0.36180905000000002</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.6203903999999998</c:v>
+                  <c:v>0.38162252000000002</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.807547</c:v>
+                  <c:v>0.35618277999999998</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.7125306</c:v>
+                  <c:v>0.36865940000000003</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.5102389999999999</c:v>
+                  <c:v>0.39836844999999999</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.6221199999999998</c:v>
+                  <c:v>0.38137080000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84896000"/>
-        <c:axId val="84910464"/>
+        <c:axId val="87063552"/>
+        <c:axId val="87069824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84896000"/>
+        <c:axId val="87063552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7661,14 +7673,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84910464"/>
+        <c:crossAx val="87069824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84910464"/>
+        <c:axId val="87069824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7685,7 +7697,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number of Papers</a:t>
+                  <a:t>Number of New Authos</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -7694,7 +7706,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84896000"/>
+        <c:crossAx val="87063552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7707,7 +7719,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -11428,7 +11440,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11458,10 +11470,10 @@
         <v>1969</v>
       </c>
       <c r="B2">
-        <v>2.5333332999999998</v>
+        <v>0.39473686000000002</v>
       </c>
       <c r="C2">
-        <v>2.5333332999999998</v>
+        <v>0.39473686000000002</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -11469,10 +11481,10 @@
         <v>1970</v>
       </c>
       <c r="B3">
-        <v>2.3199999999999998</v>
+        <v>0.43103448</v>
       </c>
       <c r="C3">
-        <v>2.3199999999999998</v>
+        <v>0.43103448</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -11480,10 +11492,10 @@
         <v>1971</v>
       </c>
       <c r="B4">
-        <v>2.5454545</v>
+        <v>0.39285713</v>
       </c>
       <c r="C4">
-        <v>2.5454545</v>
+        <v>0.39285713</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -11491,10 +11503,10 @@
         <v>1972</v>
       </c>
       <c r="B5">
-        <v>2.8333333000000001</v>
+        <v>0.35294120000000001</v>
       </c>
       <c r="C5">
-        <v>2.8333333000000001</v>
+        <v>0.35294120000000001</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -11502,10 +11514,10 @@
         <v>1973</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>0.33333333999999998</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>0.33333333999999998</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -11513,10 +11525,10 @@
         <v>1974</v>
       </c>
       <c r="B7">
-        <v>2.6119403999999999</v>
+        <v>0.38285713999999998</v>
       </c>
       <c r="C7">
-        <v>2.6666666999999999</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -11524,10 +11536,10 @@
         <v>1975</v>
       </c>
       <c r="B8">
-        <v>2.3797470000000001</v>
+        <v>0.42021278000000001</v>
       </c>
       <c r="C8">
-        <v>2.2999999999999998</v>
+        <v>0.43478260000000002</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -11535,10 +11547,10 @@
         <v>1976</v>
       </c>
       <c r="B9">
-        <v>2.5</v>
+        <v>0.4</v>
       </c>
       <c r="C9">
-        <v>2.4375</v>
+        <v>0.41025642000000001</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -11546,10 +11558,10 @@
         <v>1977</v>
       </c>
       <c r="B10">
-        <v>2.4729728999999998</v>
+        <v>0.4043716</v>
       </c>
       <c r="C10">
-        <v>2.3714284999999999</v>
+        <v>0.42168674</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -11557,10 +11569,10 @@
         <v>1978</v>
       </c>
       <c r="B11">
-        <v>2.8985506999999999</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="C11">
-        <v>2.7938930000000002</v>
+        <v>0.35792350000000001</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -11568,10 +11580,10 @@
         <v>1979</v>
       </c>
       <c r="B12">
-        <v>2.8993289999999998</v>
+        <v>0.34490739999999998</v>
       </c>
       <c r="C12">
-        <v>2.8095238</v>
+        <v>0.35593219999999998</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -11579,10 +11591,10 @@
         <v>1980</v>
       </c>
       <c r="B13">
-        <v>3.0722222000000001</v>
+        <v>0.32549729999999999</v>
       </c>
       <c r="C13">
-        <v>3.0620154999999998</v>
+        <v>0.32658228</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -11590,16 +11602,16 @@
         <v>1981</v>
       </c>
       <c r="B14">
-        <v>2.8049792999999998</v>
+        <v>0.35650887999999997</v>
       </c>
       <c r="C14">
-        <v>3.0337079</v>
+        <v>0.32962963000000001</v>
       </c>
       <c r="D14">
-        <v>2.1458333000000001</v>
+        <v>0.46601942000000002</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -11607,16 +11619,16 @@
         <v>1982</v>
       </c>
       <c r="B15">
-        <v>3.2352940000000001</v>
+        <v>0.3090909</v>
       </c>
       <c r="C15">
-        <v>3.2479339</v>
+        <v>0.30788802999999998</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>2.1724138000000002</v>
+        <v>0.46031746000000001</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -11624,13 +11636,13 @@
         <v>1983</v>
       </c>
       <c r="B16">
-        <v>2.9969969000000001</v>
+        <v>0.33366733999999998</v>
       </c>
       <c r="C16">
-        <v>2.9761905999999998</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="D16">
-        <v>2.5211266999999999</v>
+        <v>0.39664804999999997</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -11641,16 +11653,16 @@
         <v>1984</v>
       </c>
       <c r="B17">
-        <v>2.9864407000000002</v>
+        <v>0.33484676000000002</v>
       </c>
       <c r="C17">
-        <v>2.8278690000000002</v>
+        <v>0.35362317999999998</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>2.2142856000000002</v>
+        <v>0.45161289999999998</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -11658,16 +11670,16 @@
         <v>1985</v>
       </c>
       <c r="B18">
-        <v>3.2357724000000001</v>
+        <v>0.30904523</v>
       </c>
       <c r="C18">
-        <v>3.4361700000000002</v>
+        <v>0.29102167000000001</v>
       </c>
       <c r="D18">
-        <v>2.2045455</v>
+        <v>0.45360824</v>
       </c>
       <c r="E18">
-        <v>2.4137930000000001</v>
+        <v>0.41428572000000002</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -11675,19 +11687,19 @@
         <v>1986</v>
       </c>
       <c r="B19">
-        <v>3.3765903000000002</v>
+        <v>0.29615672999999998</v>
       </c>
       <c r="C19">
-        <v>3.3317757000000001</v>
+        <v>0.30014025999999999</v>
       </c>
       <c r="D19">
-        <v>2.3131312999999998</v>
+        <v>0.43231439999999999</v>
       </c>
       <c r="E19">
-        <v>2.3333333000000001</v>
+        <v>0.42857142999999998</v>
       </c>
       <c r="F19">
-        <v>2.0238094000000002</v>
+        <v>0.49411765000000002</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -11695,19 +11707,19 @@
         <v>1987</v>
       </c>
       <c r="B20">
-        <v>3.3246074000000001</v>
+        <v>0.30078739999999998</v>
       </c>
       <c r="C20">
-        <v>3.3130841000000002</v>
+        <v>0.30183357</v>
       </c>
       <c r="D20">
-        <v>2.0909089999999999</v>
+        <v>0.47826087</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
-        <v>2.1666666999999999</v>
+        <v>0.46153845999999998</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -11715,19 +11727,19 @@
         <v>1988</v>
       </c>
       <c r="B21">
-        <v>3.4949083000000001</v>
+        <v>0.28613054999999998</v>
       </c>
       <c r="C21">
-        <v>3.521531</v>
+        <v>0.28396739999999998</v>
       </c>
       <c r="D21">
-        <v>2.3368419999999999</v>
+        <v>0.42792794000000001</v>
       </c>
       <c r="E21">
-        <v>2.2666667</v>
+        <v>0.44117646999999999</v>
       </c>
       <c r="F21">
-        <v>2.4166666999999999</v>
+        <v>0.41379312000000001</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -11735,19 +11747,19 @@
         <v>1989</v>
       </c>
       <c r="B22">
-        <v>3.8297362000000001</v>
+        <v>0.26111459999999997</v>
       </c>
       <c r="C22">
-        <v>4.0598802999999997</v>
+        <v>0.24631268000000001</v>
       </c>
       <c r="D22">
-        <v>2.3441296</v>
+        <v>0.42659760000000002</v>
       </c>
       <c r="E22">
-        <v>2.0754716000000002</v>
+        <v>0.48181816999999999</v>
       </c>
       <c r="F22">
-        <v>2.4166666999999999</v>
+        <v>0.41379312000000001</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -11755,16 +11767,16 @@
         <v>1990</v>
       </c>
       <c r="B23">
-        <v>3.5036900000000002</v>
+        <v>0.28541337999999999</v>
       </c>
       <c r="C23">
-        <v>4.2848835000000003</v>
+        <v>0.23337856000000001</v>
       </c>
       <c r="D23">
-        <v>2.3682432000000002</v>
+        <v>0.42225393999999999</v>
       </c>
       <c r="E23">
-        <v>2.347826</v>
+        <v>0.42592594</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -11775,19 +11787,19 @@
         <v>1991</v>
       </c>
       <c r="B24">
-        <v>3.4951612999999999</v>
+        <v>0.28610983000000001</v>
       </c>
       <c r="C24">
-        <v>3.8038278000000001</v>
+        <v>0.26289308</v>
       </c>
       <c r="D24">
-        <v>2.4735203000000001</v>
+        <v>0.40428212000000002</v>
       </c>
       <c r="E24">
-        <v>2.2109375</v>
+        <v>0.45229681999999999</v>
       </c>
       <c r="F24">
-        <v>2.58</v>
+        <v>0.38759690000000002</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -11795,19 +11807,19 @@
         <v>1992</v>
       </c>
       <c r="B25">
-        <v>3.5219939999999998</v>
+        <v>0.28393005999999998</v>
       </c>
       <c r="C25">
-        <v>3.9414634999999998</v>
+        <v>0.25371285999999998</v>
       </c>
       <c r="D25">
-        <v>2.5269841999999998</v>
+        <v>0.39572865000000002</v>
       </c>
       <c r="E25">
-        <v>2.2424241999999999</v>
+        <v>0.44594594999999998</v>
       </c>
       <c r="F25">
-        <v>2.4264705000000002</v>
+        <v>0.41212120000000002</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -11815,19 +11827,19 @@
         <v>1993</v>
       </c>
       <c r="B26">
-        <v>3.5569334000000001</v>
+        <v>0.28114104000000001</v>
       </c>
       <c r="C26">
-        <v>3.7456445999999999</v>
+        <v>0.26697673999999999</v>
       </c>
       <c r="D26">
-        <v>2.5955284000000001</v>
+        <v>0.38527800000000001</v>
       </c>
       <c r="E26">
-        <v>2.2962964000000001</v>
+        <v>0.43548387</v>
       </c>
       <c r="F26">
-        <v>2.8666665999999998</v>
+        <v>0.34883720000000001</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -11835,19 +11847,19 @@
         <v>1994</v>
       </c>
       <c r="B27">
-        <v>3.5356394999999998</v>
+        <v>0.28283426</v>
       </c>
       <c r="C27">
-        <v>3.8357142999999998</v>
+        <v>0.26070765000000001</v>
       </c>
       <c r="D27">
-        <v>2.6808510000000001</v>
+        <v>0.37301588000000002</v>
       </c>
       <c r="E27">
-        <v>2.5</v>
+        <v>0.4</v>
       </c>
       <c r="F27">
-        <v>2.359375</v>
+        <v>0.42384105999999999</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -11855,19 +11867,19 @@
         <v>1995</v>
       </c>
       <c r="B28">
-        <v>3.6125702999999998</v>
+        <v>0.27681119999999998</v>
       </c>
       <c r="C28">
-        <v>3.6088328000000001</v>
+        <v>0.27709790000000001</v>
       </c>
       <c r="D28">
-        <v>3.0216799999999999</v>
+        <v>0.33094170000000001</v>
       </c>
       <c r="E28">
-        <v>2.4976959999999999</v>
+        <v>0.40036902000000002</v>
       </c>
       <c r="F28">
-        <v>2.3880596000000001</v>
+        <v>0.41875000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -11875,19 +11887,19 @@
         <v>1996</v>
       </c>
       <c r="B29">
-        <v>3.7420814</v>
+        <v>0.26723096000000002</v>
       </c>
       <c r="C29">
-        <v>3.9520547000000001</v>
+        <v>0.25303291999999999</v>
       </c>
       <c r="D29">
-        <v>2.9225807000000001</v>
+        <v>0.34216334999999998</v>
       </c>
       <c r="E29">
-        <v>2.5</v>
+        <v>0.4</v>
       </c>
       <c r="F29">
-        <v>2.4396550000000001</v>
+        <v>0.40989399999999998</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -11895,19 +11907,19 @@
         <v>1997</v>
       </c>
       <c r="B30">
-        <v>3.635767</v>
+        <v>0.27504513000000003</v>
       </c>
       <c r="C30">
-        <v>3.9255664000000001</v>
+        <v>0.25474033000000001</v>
       </c>
       <c r="D30">
-        <v>2.7206106000000001</v>
+        <v>0.36756453</v>
       </c>
       <c r="E30">
-        <v>2.4285714999999999</v>
+        <v>0.41176469999999998</v>
       </c>
       <c r="F30">
-        <v>2.6129030000000002</v>
+        <v>0.38271606000000002</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -11915,19 +11927,19 @@
         <v>1998</v>
       </c>
       <c r="B31">
-        <v>3.7050242</v>
+        <v>0.26990375</v>
       </c>
       <c r="C31">
-        <v>3.9788519999999998</v>
+        <v>0.25132876999999998</v>
       </c>
       <c r="D31">
-        <v>2.9703154999999999</v>
+        <v>0.33666459999999998</v>
       </c>
       <c r="E31">
-        <v>2.7363183000000002</v>
+        <v>0.36545454999999999</v>
       </c>
       <c r="F31">
-        <v>2.4122447999999999</v>
+        <v>0.41455162000000001</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -11935,19 +11947,19 @@
         <v>1999</v>
       </c>
       <c r="B32">
-        <v>3.8543753999999999</v>
+        <v>0.25944539999999999</v>
       </c>
       <c r="C32">
-        <v>4.0144929999999999</v>
+        <v>0.24909746999999999</v>
       </c>
       <c r="D32">
-        <v>2.9848275000000002</v>
+        <v>0.33502771999999997</v>
       </c>
       <c r="E32">
-        <v>2.4570637</v>
+        <v>0.40698983999999999</v>
       </c>
       <c r="F32">
-        <v>2.6898735</v>
+        <v>0.37176471999999999</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -11955,19 +11967,19 @@
         <v>2000</v>
       </c>
       <c r="B33">
-        <v>3.6032926999999999</v>
+        <v>0.27752396000000001</v>
       </c>
       <c r="C33">
-        <v>3.8223684000000002</v>
+        <v>0.26161790000000001</v>
       </c>
       <c r="D33">
-        <v>3.0013036999999998</v>
+        <v>0.33318852999999998</v>
       </c>
       <c r="E33">
-        <v>2.7349079999999999</v>
+        <v>0.365643</v>
       </c>
       <c r="F33">
-        <v>2.5423453</v>
+        <v>0.39333760000000001</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -11975,19 +11987,19 @@
         <v>2001</v>
       </c>
       <c r="B34">
-        <v>3.7321996999999998</v>
+        <v>0.26793850000000002</v>
       </c>
       <c r="C34">
-        <v>3.6928570000000001</v>
+        <v>0.27079304999999998</v>
       </c>
       <c r="D34">
-        <v>3.0252100999999998</v>
+        <v>0.33055556000000003</v>
       </c>
       <c r="E34">
-        <v>2.8286853000000001</v>
+        <v>0.35352114000000001</v>
       </c>
       <c r="F34">
-        <v>2.6825937999999998</v>
+        <v>0.37277353000000002</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -11995,19 +12007,19 @@
         <v>2002</v>
       </c>
       <c r="B35">
-        <v>3.8033332999999998</v>
+        <v>0.26292726</v>
       </c>
       <c r="C35">
-        <v>3.7221375000000001</v>
+        <v>0.26866284000000001</v>
       </c>
       <c r="D35">
-        <v>2.9572023999999999</v>
+        <v>0.33815741999999999</v>
       </c>
       <c r="E35">
-        <v>2.7438015999999998</v>
+        <v>0.36445785000000003</v>
       </c>
       <c r="F35">
-        <v>2.5450081999999998</v>
+        <v>0.39292603999999998</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -12015,19 +12027,19 @@
         <v>2003</v>
       </c>
       <c r="B36">
-        <v>3.6797065999999998</v>
+        <v>0.27176080000000002</v>
       </c>
       <c r="C36">
-        <v>3.8064515999999999</v>
+        <v>0.26271185000000002</v>
       </c>
       <c r="D36">
-        <v>2.9024165000000002</v>
+        <v>0.34454050000000003</v>
       </c>
       <c r="E36">
-        <v>2.8690095000000002</v>
+        <v>0.34855235000000001</v>
       </c>
       <c r="F36">
-        <v>2.4640521999999998</v>
+        <v>0.40583553999999999</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -12035,19 +12047,19 @@
         <v>2004</v>
       </c>
       <c r="B37">
-        <v>3.8127870000000001</v>
+        <v>0.26227534000000002</v>
       </c>
       <c r="C37">
-        <v>3.9075066999999999</v>
+        <v>0.25591766999999999</v>
       </c>
       <c r="D37">
-        <v>3.0810168</v>
+        <v>0.32456817999999998</v>
       </c>
       <c r="E37">
-        <v>2.7867434000000002</v>
+        <v>0.35884178</v>
       </c>
       <c r="F37">
-        <v>2.6584506000000001</v>
+        <v>0.37615894999999999</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -12055,19 +12067,19 @@
         <v>2005</v>
       </c>
       <c r="B38">
-        <v>3.8323269999999998</v>
+        <v>0.26093808000000002</v>
       </c>
       <c r="C38">
-        <v>3.5622745</v>
+        <v>0.28071954999999998</v>
       </c>
       <c r="D38">
-        <v>3.1145339999999999</v>
+        <v>0.32107532</v>
       </c>
       <c r="E38">
-        <v>2.7741935</v>
+        <v>0.36046509999999998</v>
       </c>
       <c r="F38">
-        <v>2.6355422000000002</v>
+        <v>0.37942857000000002</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -12075,19 +12087,19 @@
         <v>2006</v>
       </c>
       <c r="B39">
-        <v>3.9104682999999998</v>
+        <v>0.25572382999999999</v>
       </c>
       <c r="C39">
-        <v>3.4588679999999998</v>
+        <v>0.28911194000000001</v>
       </c>
       <c r="D39">
-        <v>3.2113269999999998</v>
+        <v>0.31139772999999998</v>
       </c>
       <c r="E39">
-        <v>2.9435897</v>
+        <v>0.33972126000000002</v>
       </c>
       <c r="F39">
-        <v>2.4810894000000001</v>
+        <v>0.40304878</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -12095,19 +12107,19 @@
         <v>2007</v>
       </c>
       <c r="B40">
-        <v>3.8405306000000001</v>
+        <v>0.26038070000000002</v>
       </c>
       <c r="C40">
-        <v>3.8999079999999999</v>
+        <v>0.25641629999999999</v>
       </c>
       <c r="D40">
-        <v>2.9588087000000001</v>
+        <v>0.33797386000000001</v>
       </c>
       <c r="E40">
-        <v>2.8509316</v>
+        <v>0.35076252000000002</v>
       </c>
       <c r="F40">
-        <v>2.6284290000000001</v>
+        <v>0.3804554</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -12115,19 +12127,19 @@
         <v>2008</v>
       </c>
       <c r="B41">
-        <v>4.1850265999999996</v>
+        <v>0.2389471</v>
       </c>
       <c r="C41">
-        <v>4.015625</v>
+        <v>0.24902724000000001</v>
       </c>
       <c r="D41">
-        <v>3.215856</v>
+        <v>0.31095919999999999</v>
       </c>
       <c r="E41">
-        <v>2.9965869999999999</v>
+        <v>0.33371299999999998</v>
       </c>
       <c r="F41">
-        <v>2.7638888000000001</v>
+        <v>0.36180905000000002</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -12135,19 +12147,19 @@
         <v>2009</v>
       </c>
       <c r="B42">
-        <v>4.0149125999999997</v>
+        <v>0.24907141999999999</v>
       </c>
       <c r="C42">
-        <v>3.8560688000000001</v>
+        <v>0.25933146000000001</v>
       </c>
       <c r="D42">
-        <v>3.3525143000000002</v>
+        <v>0.29828359999999998</v>
       </c>
       <c r="E42">
-        <v>2.8507042</v>
+        <v>0.35079050000000001</v>
       </c>
       <c r="F42">
-        <v>2.6203903999999998</v>
+        <v>0.38162252000000002</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -12155,19 +12167,19 @@
         <v>2010</v>
       </c>
       <c r="B43">
-        <v>4.0448979999999999</v>
+        <v>0.24722503000000001</v>
       </c>
       <c r="C43">
-        <v>3.6157205000000001</v>
+        <v>0.27657005000000001</v>
       </c>
       <c r="D43">
-        <v>3.3944223</v>
+        <v>0.29460092999999998</v>
       </c>
       <c r="E43">
-        <v>2.7142856000000002</v>
+        <v>0.36842105000000003</v>
       </c>
       <c r="F43">
-        <v>2.807547</v>
+        <v>0.35618277999999998</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -12175,19 +12187,19 @@
         <v>2011</v>
       </c>
       <c r="B44">
-        <v>4.0649569999999997</v>
+        <v>0.24600504000000001</v>
       </c>
       <c r="C44">
-        <v>3.6031599999999999</v>
+        <v>0.27753420000000001</v>
       </c>
       <c r="D44">
-        <v>3.4844176999999998</v>
+        <v>0.28699197999999998</v>
       </c>
       <c r="E44">
-        <v>3</v>
+        <v>0.33333333999999998</v>
       </c>
       <c r="F44">
-        <v>2.7125306</v>
+        <v>0.36865940000000003</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -12195,19 +12207,19 @@
         <v>2012</v>
       </c>
       <c r="B45">
-        <v>3.8371559999999998</v>
+        <v>0.2606097</v>
       </c>
       <c r="C45">
-        <v>3.4646466</v>
+        <v>0.28862974000000002</v>
       </c>
       <c r="D45">
-        <v>3.4211566000000002</v>
+        <v>0.29229880000000003</v>
       </c>
       <c r="E45">
-        <v>2.7975078</v>
+        <v>0.35746104000000001</v>
       </c>
       <c r="F45">
-        <v>2.5102389999999999</v>
+        <v>0.39836844999999999</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -12215,19 +12227,19 @@
         <v>2013</v>
       </c>
       <c r="B46">
-        <v>3.9621474999999999</v>
+        <v>0.25238840000000001</v>
       </c>
       <c r="C46">
-        <v>3.6183866999999998</v>
+        <v>0.27636625999999997</v>
       </c>
       <c r="D46">
-        <v>3.5429417999999999</v>
+        <v>0.28225133000000002</v>
       </c>
       <c r="E46">
-        <v>2.8410852000000002</v>
+        <v>0.35197817999999997</v>
       </c>
       <c r="F46">
-        <v>2.6221199999999998</v>
+        <v>0.38137080000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>